<commit_message>
Added create year table
</commit_message>
<xml_diff>
--- a/bulletin/macroeconomics/static/macroeconomics/tables/consumer_price_index1.xlsx
+++ b/bulletin/macroeconomics/static/macroeconomics/tables/consumer_price_index1.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:W7"/>
+  <dimension ref="A1:V7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -544,11 +544,6 @@
           <t>авг</t>
         </is>
       </c>
-      <c r="W2" t="inlineStr">
-        <is>
-          <t>сен</t>
-        </is>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -619,9 +614,6 @@
       <c r="V3" t="n">
         <v>113.1</v>
       </c>
-      <c r="W3" t="n">
-        <v>111.8</v>
-      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -692,9 +684,6 @@
       <c r="V4" t="n">
         <v>112.4</v>
       </c>
-      <c r="W4" t="n">
-        <v>111.4</v>
-      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -765,9 +754,6 @@
       <c r="V5" t="n">
         <v>113.5</v>
       </c>
-      <c r="W5" t="n">
-        <v>112.1</v>
-      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -838,9 +824,6 @@
       <c r="V6" t="n">
         <v>113.9</v>
       </c>
-      <c r="W6" t="n">
-        <v>111.9</v>
-      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -911,13 +894,12 @@
       <c r="V7" t="n">
         <v>92.3</v>
       </c>
-      <c r="W7" t="inlineStr"/>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B1"/>
     <mergeCell ref="C1:N1"/>
-    <mergeCell ref="O1:W1"/>
+    <mergeCell ref="O1:V1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>